<commit_message>
updated home page tests
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/TC_Login_001_AsASuperUser_PurchaseAgent_GeneralUser.xlsx
+++ b/resources/ExcelsheetData/TC_Login_001_AsASuperUser_PurchaseAgent_GeneralUser.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\etna\resources\ExcelsheetData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\Etna\resources\ExcelsheetData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>password</t>
   </si>
@@ -75,25 +75,28 @@
     <t>003</t>
   </si>
   <si>
-    <t>webuser@unilogcorp.com</t>
-  </si>
-  <si>
     <t>123456789</t>
   </si>
   <si>
     <t>newpurchaseagent@unilogcorp.com</t>
   </si>
   <si>
-    <t>generaluser2@unilogcorp.com</t>
-  </si>
-  <si>
     <t>Super User User</t>
   </si>
   <si>
     <t>Test Agent Test</t>
   </si>
   <si>
-    <t>General User Test User</t>
+    <t>hemanthgeneraluser@unilogcorp.com</t>
+  </si>
+  <si>
+    <t>hemanth123</t>
+  </si>
+  <si>
+    <t>hemanth.bs123@unilogcorp.com</t>
+  </si>
+  <si>
+    <t>Purchase Agent</t>
   </si>
 </sst>
 </file>
@@ -484,12 +487,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
   </cols>
@@ -513,27 +516,27 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -541,21 +544,20 @@
         <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bugs regarding response from ERP
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/TC_Login_001_AsASuperUser_PurchaseAgent_GeneralUser.xlsx
+++ b/resources/ExcelsheetData/TC_Login_001_AsASuperUser_PurchaseAgent_GeneralUser.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>password</t>
   </si>
@@ -63,9 +63,6 @@
     <t>userName</t>
   </si>
   <si>
-    <t>Expected</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -75,18 +72,6 @@
     <t>003</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>newpurchaseagent@unilogcorp.com</t>
-  </si>
-  <si>
-    <t>Super User User</t>
-  </si>
-  <si>
-    <t>Test Agent Test</t>
-  </si>
-  <si>
     <t>hemanthgeneraluser@unilogcorp.com</t>
   </si>
   <si>
@@ -96,14 +81,26 @@
     <t>hemanth.bs123@unilogcorp.com</t>
   </si>
   <si>
-    <t>Purchase Agent</t>
+    <t>General User User</t>
+  </si>
+  <si>
+    <t>Test Fn Test Ln</t>
+  </si>
+  <si>
+    <t>Expected Name</t>
+  </si>
+  <si>
+    <t>Hemanth Sridhar</t>
+  </si>
+  <si>
+    <t>hemanthtestapa@unilogcorp.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +120,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,23 +185,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -487,7 +500,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,66 +511,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>